<commit_message>
plot function, full generation
</commit_message>
<xml_diff>
--- a/languageGP/test_problems/problem_1adf.xlsx
+++ b/languageGP/test_problems/problem_1adf.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data.xlsx" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data.xlsx" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,10 +426,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>512251.0721023057</v>
+        <v>63471.86276619376</v>
       </c>
       <c r="C1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -437,10 +437,1088 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>577.6320767246821</v>
+        <v>20.21599999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>5</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>9</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>8.960800000000001</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.2943999999999997</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>8.059200000000001</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
+        <v>8.059200000000001</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
+        <v>4.0592</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
+        <v>4.059200000000001</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
+        <v>4.059200000000001</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.02000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>